<commit_message>
working optimizer and datasets
</commit_message>
<xml_diff>
--- a/python/input.xlsx
+++ b/python/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/EvTransitMatsim/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697F7817-1B3F-A141-A8CE-2BF0C4ABA5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0F7A0E-E42F-6043-84A2-88EF465A785D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -892,9 +892,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A97"/>
+  <dimension ref="A1:A111"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1386,6 +1388,70 @@
         <v>0.101522404371585</v>
       </c>
     </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>9.6196376021798397E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>9.6196376021798397E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>9.6196376021798397E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>9.6196376021798397E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>8.8765994550408706E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>8.8765994550408706E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>8.8765994550408706E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>8.8765994550408706E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>8.4496621253405998E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>8.4496621253405998E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>8.4496621253405998E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>